<commit_message>
descriptions of our 5 cities
</commit_message>
<xml_diff>
--- a/5_cities_descriptions .xlsx
+++ b/5_cities_descriptions .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Picture</t>
   </si>
   <si>
-    <t>Tokyo ( Japan)</t>
-  </si>
-  <si>
     <t>Temperate</t>
   </si>
   <si>
@@ -102,16 +99,52 @@
     <t>Seoul, South Korea</t>
   </si>
   <si>
-    <t>Sevilla, Capital of Andalousia, South of Spain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capital of Japan </t>
-  </si>
-  <si>
     <t xml:space="preserve">Rio is the second biggest city of Brazil </t>
   </si>
   <si>
-    <t>Capital of Italy</t>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokyo </t>
+  </si>
+  <si>
+    <t>Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro, Brazil</t>
+  </si>
+  <si>
+    <t>Rome, Italy</t>
+  </si>
+  <si>
+    <t>Seville, Spain</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Flag_of_Japan#/media/File:Flag_of_Japan.svg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Flag_of_Brazil#/media/File:Flag_of_Brazil.svg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Flag_of_Italy#/media/File:Flag_of_Italy.svg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Flag_of_South_Korea#/media/File:Flag_of_South_Korea.svg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Flag_of_Spain#/media/File:Flag_of_Spain.svg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yens </t>
+  </si>
+  <si>
+    <t>Euro</t>
+  </si>
+  <si>
+    <t>Brazilian real</t>
+  </si>
+  <si>
+    <t>South Korean Won</t>
   </si>
 </sst>
 </file>
@@ -173,7 +206,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
@@ -186,6 +219,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -520,149 +557,188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H10"/>
+  <dimension ref="B3:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="34.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="32" customHeight="1">
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="45">
-      <c r="B5" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="32" customHeight="1">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" t="s">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:8" ht="47" customHeight="1">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
everythig to know about our 5 cities
</commit_message>
<xml_diff>
--- a/5_cities_descriptions .xlsx
+++ b/5_cities_descriptions .xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$3:$H$11</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -51,9 +54,6 @@
     <t>Temperate</t>
   </si>
   <si>
-    <t>Tokyo is Japan's capital and the world's most populous metropolis</t>
-  </si>
-  <si>
     <t>GMT+9 ( Greenwich Mean Time)</t>
   </si>
   <si>
@@ -78,9 +78,6 @@
     <t>GMT +1</t>
   </si>
   <si>
-    <t>Italy's capital</t>
-  </si>
-  <si>
     <t>Seoul</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Seoul, South Korea</t>
   </si>
   <si>
-    <t xml:space="preserve">Rio is the second biggest city of Brazil </t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>Seville, Spain</t>
   </si>
   <si>
-    <t>https://en.wikipedia.org/wiki/Flag_of_Japan#/media/File:Flag_of_Japan.svg</t>
-  </si>
-  <si>
     <t>https://en.wikipedia.org/wiki/Flag_of_Brazil#/media/File:Flag_of_Brazil.svg</t>
   </si>
   <si>
@@ -135,9 +126,6 @@
     <t>https://en.wikipedia.org/wiki/Flag_of_Spain#/media/File:Flag_of_Spain.svg</t>
   </si>
   <si>
-    <t xml:space="preserve">Yens </t>
-  </si>
-  <si>
     <t>Euro</t>
   </si>
   <si>
@@ -145,13 +133,683 @@
   </si>
   <si>
     <t>South Korean Won</t>
+  </si>
+  <si>
+    <t>Yen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tokyo, skyscrapers modernity and tradition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;                                 &lt;img class="irc_mi" src="https://www.challenges.fr/assets/img/2012/06/21/cover-r4x3w1000-5b2d1f42956fe-vue-du-mont-fuji-dominant-l-arrondissement-de-shinjuku-a.jpg" data-atf="0" style="" alt="Image associée" width="499" height="374"&gt;                                                       2&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tokyo, lights buildings games</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;                                                          &lt;img data-src="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTo-Vy4I2dXefXTNP7SA4z3-E-Gmczby9bKb7GKjeUia_FSP4lwDw&amp;amp;s" jsaction="load:str.tbn" class="rg_ic rg_i" alt="Résultat de recherche d'images pour &amp;quot;tokyo lights buildings&amp;quot;" onload="typeof google==='object'&amp;amp;&amp;amp;google.aft&amp;amp;&amp;amp;google.aft(this)" style="width: 279px; height: 181px; margin-left: 8px; margin-right: 8px; margin-top: -8px;" src="https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTo-Vy4I2dXefXTNP7SA4z3-E-Gmczby9bKb7GKjeUia_FSP4lwDw&amp;amp;s"&gt;                                                                                                                   3&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Tokyo, temples and cherry blossoms </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;&gt;              src="https://www.lonelyplanet.com/news/wp-content/uploads/2019/01/cherry-blossoms-sakura.jpg"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rio, Christ Corcovado mountains</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;                                               &lt;img src="https://viago.ca/wp-content/uploads/2017/10/Incontournables_rio-768x432.jpg" alt="10 incontournables à Rio de Janeiro" class="img-responsive"&gt;                                                                     2&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rio, carnaval de rio de janeiro</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  &gt;&gt; src="https://media.tacdn.com/media/attractions-splice-spp-674x446/06/73/dc/13.jpg"                                                                          3&gt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Rio, beaches Ipanema Copacabana</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;         src="https://spotlight.it-notes.ru/wp-content/uploads/2018/01/1b0dc1fb3e94546119242b37725d0c6c.jpg"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1&gt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Colosseum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;&gt; https://img.lemde.fr/2019/04/15/41/0/500/333/688/0/60/0/875bc88_4S376NSwaGX_d8P5dfgCYl5c.jpg                       2&gt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rome, Roman forum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt; &lt;img class="irc_mi" src="https://traveladestatic.imgix.net/media/image/colosseum-roman-forum-palatine-hill-skip-the-lines-tour_276822_1ERF9bK.jpg?fit=crop&amp;amp;w=1200&amp;amp;h=630" alt="Résultat de recherche d'images pour &amp;quot;roman forum&amp;quot;" width="450" height="236" style="&gt;                                                          3&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rome, Trevi fountain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt; src="https://miro.medium.com/max/700/1*4okBZucF2oNu3SAEvgL3MA.jpeg"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seoul, architecture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt; src="https://www.ef.com/blog/wp-content/uploads/2017/09/Visit_Seoul_web.jpg"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1&gt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Seville,Alcazar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt; style="background-position: center center; background-image: url("https://cdn.getyourguide.com/img/tour_img-1098570-99.jpg");"</t>
+    </r>
+  </si>
+  <si>
+    <t>Tokyo is Japan's capital and the world's most populous .Tokyo is considered to be one of the world's most important and powerful global cities.</t>
+  </si>
+  <si>
+    <t>Rio is anchor to the Rio de Janeiro metropolitan area and the second-most populous municipality in Brazil and the sixth-most populous in the Americas. Rio de Janeiro is the capital of the state of Rio de Janeiro, Brazil's third-most populous state.</t>
+  </si>
+  <si>
+    <t>Rome is the capital city and a special comune of Italy.Rome also serves as the capital of the Lazio region.</t>
+  </si>
+  <si>
+    <t>Seoul officially the Seoul Special City, is the capital and largest metropolis of South Korea. With surrounding Incheon metropolis and Gyeonggi province, Seoul forms the heart of the Seoul Capital Area</t>
+  </si>
+  <si>
+    <t>Seville, is a Spanish city, the capital of the autonomous community of Andalusia and the province of Seville. It is situated on the lower reaches of the River Guadalquivir, in the southwest of the Iberian Peninsula</t>
+  </si>
+  <si>
+    <r>
+      <t>&gt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sports</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;&gt;                                                                                                           In Japan</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sumo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is much more than just a sport. It is a living example of Japanese culture, traditions and history. And the rikishi or wrestlers serve as cultural ambassadors when they take part in events overseas.
+Sumo shows discipline, hard work and courage but not only inside the dohyō or ring, also outside and in wrestlers´ every day life.                     &gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Religion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt;                                                                                                     there are two main religions in Japan: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shinto and Buddhism</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.                 &gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Food</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt;                                                                                                    Across the nation, the Japanese are primarily fish eaters. Japan is the number one fish importer in the world, consuming around 12% of the world’s caught fish.
+The most well-known Japanese dish is probably </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sushi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, a dish that includes fresh fish, seaweed and lightly-seasoned rice. Japanese also eat beef, poultry and pork as part of their daily diets.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sports</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;                                                                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Carnaval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, the traditional festival of decadence before Lent begins, has some of its biggest celebrations in Brazil.                                                </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Football</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Brazilians probably know the true passion football brings more than almost any other country. Everyone from men and women to children will usually have a team and football stadiums become charged with emotions as rival teams from across the country battle it out on the pitch to the sound of thousands of fans cheering, booing and singing.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Food</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt;                                                                                                                              </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Supplì</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Any Roman will agree, the best way to whet your appetite before digging into a personal pizza is with fritti: deep-fried goodies that are tasty, comforting and oh-so-satisfying. A classic choice is the supplì, a fried rice-ball mixed with ragù and mozzarella and cooked to perfection.                                                                           </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF800000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bucatini all’Amatriciana</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ,at Da Bucatino
+Amatriciana is another favorite: this tomato-based pasta also features crispy guanciale (cured pork jowl) and is typically served with bucatini noodles, which are similar to thicker, hollow spaghetti.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Culture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;                                                  Korea is greatly influenced by the Chinese and Japanese cultures. This influence can be seen by Confucianism, which established many traditions that can be seen in modern Korea today. These traditions include the ethical code of conduct in social life and showing respect to the elders and family.    &gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Food</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&gt;&gt;                                                      Korean cuisine is largely based on rice, noodles, vegetables and meats. Some of the famous Korean dishes include bibimbap, bulgogi and dakgalbi. The Korean culture is based on politeness and respect and this is clearly evident in Korean table manners.     &gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Music</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;                                                        K-pop is a musical genre originating in South Korea, characterized by a wide variety of audiovisual elements. Although it incorporates all forms of Korean popular music, such as trot and folk music, the term is more often used to refer to songs produced by idol groups</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&gt;&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Holy Week</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.&gt;&gt;                                                     During the Holy Week in Seville, the city recovers a tradition that has been celebrated since Roman times. In these days, religion and history go hand in hand. Many of the streets of Seville are filled with processions - or religious parades - to carry the crucifix of Jesus Christ or virgins and saints.                                                    &gt;&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La Bienal de Flamenco</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt;
+The Bienal de Flamenco is an internationally known flamenco festival born in 1980. It is organized every two years, hence its name, between the months of September and October in Seville. Singing, guitar and dancing activities are organized in places around the city, such as the Teatro de la Maestranza, the Teatro Lope de Vega and Plaza de Toros de la Real and many others</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -183,6 +841,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,11 +901,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -223,6 +915,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -559,68 +1266,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="34.6640625" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="58.6640625" customWidth="1"/>
+    <col min="5" max="5" width="56.5" customWidth="1"/>
     <col min="6" max="6" width="35.1640625" customWidth="1"/>
     <col min="7" max="7" width="37" customWidth="1"/>
     <col min="8" max="8" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="32" customHeight="1">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="5" t="s">
-        <v>16</v>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -628,121 +1335,157 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>17</v>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="32" customHeight="1">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="2:8" ht="97" customHeight="1">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
+      <c r="D6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
         <v>21</v>
       </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="2:8" ht="311" customHeight="1">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="D8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="9" spans="2:8" ht="47" customHeight="1">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:8" ht="54" customHeight="1">
+      <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="2:8" ht="409" customHeight="1">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
+      <c r="D10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="5" t="s">
-        <v>27</v>
+      <c r="B11" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B3:H11"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>